<commit_message>
doc updates and tab01 updates
</commit_message>
<xml_diff>
--- a/tables/tab01.xlsx
+++ b/tables/tab01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Projekte\07-COOEE\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Projekte\07-COOEE\NLPmeetsCOOEE\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7129555-A2F7-43C3-A7BB-867308592758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C52D418-43DD-42EC-836B-9DA591876F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="3345" windowWidth="21600" windowHeight="11385" xr2:uid="{2B2B4F61-389F-4D29-9737-758F0630C4F9}"/>
+    <workbookView xWindow="3045" yWindow="1695" windowWidth="17640" windowHeight="11115" xr2:uid="{2B2B4F61-389F-4D29-9737-758F0630C4F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>Datecat</t>
   </si>
@@ -80,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,9 +92,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,13 +158,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,228 +480,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87656B72-12B5-41C1-9DD6-5F4E386125AB}">
-  <dimension ref="B1:F14"/>
+  <dimension ref="B1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2799</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4010</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D4" s="3">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3">
+        <v>11532</v>
+      </c>
+      <c r="F4" s="3">
+        <v>24225</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3">
+        <v>6595</v>
+      </c>
+      <c r="F5" s="3">
+        <v>13914</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7515</v>
+      </c>
+      <c r="F6" s="3">
+        <v>12773</v>
+      </c>
+      <c r="G6" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>57</v>
+      </c>
+      <c r="E7" s="3">
+        <v>21153</v>
+      </c>
+      <c r="F7" s="3">
+        <v>32605</v>
+      </c>
+      <c r="G7" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>52</v>
+      </c>
+      <c r="E8" s="3">
+        <v>25209</v>
+      </c>
+      <c r="F8" s="3">
+        <v>48851</v>
+      </c>
+      <c r="G8" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3">
-        <v>18033</v>
-      </c>
-      <c r="F3" s="3">
-        <v>63568</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>56</v>
+      </c>
+      <c r="E9" s="3">
+        <v>19924</v>
+      </c>
+      <c r="F9" s="3">
+        <v>33302</v>
+      </c>
+      <c r="G9" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4">
-        <v>46</v>
-      </c>
-      <c r="E4" s="4">
-        <v>33332</v>
-      </c>
-      <c r="F4" s="4">
-        <v>102608</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D10" s="3">
+        <v>61</v>
+      </c>
+      <c r="E10" s="3">
+        <v>19150</v>
+      </c>
+      <c r="F10" s="3">
+        <v>29207</v>
+      </c>
+      <c r="G10" s="6">
         <v>8</v>
       </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
-        <v>170</v>
-      </c>
-      <c r="F5" s="4">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>19</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4715</v>
+      </c>
+      <c r="F11" s="3">
+        <v>6964</v>
+      </c>
+      <c r="G11" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4">
-        <v>86</v>
-      </c>
-      <c r="E6" s="4">
-        <v>48063</v>
-      </c>
-      <c r="F6" s="4">
-        <v>114444</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="D12" s="3">
+        <v>41</v>
+      </c>
+      <c r="E12" s="3">
+        <v>17996</v>
+      </c>
+      <c r="F12" s="3">
+        <v>45283</v>
+      </c>
+      <c r="G12" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4">
-        <v>6</v>
-      </c>
-      <c r="E7" s="4">
-        <v>6858</v>
-      </c>
-      <c r="F7" s="4">
-        <v>19934</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D13" s="3">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3813</v>
+      </c>
+      <c r="F13" s="3">
+        <v>7623</v>
+      </c>
+      <c r="G13" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4">
-        <v>131</v>
-      </c>
-      <c r="E8" s="4">
-        <v>88065</v>
-      </c>
-      <c r="F8" s="4">
-        <v>213955</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4">
-        <v>6576</v>
-      </c>
-      <c r="F9" s="4">
-        <v>17965</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>33</v>
-      </c>
-      <c r="E10" s="4">
-        <v>29876</v>
-      </c>
-      <c r="F10" s="4">
-        <v>74056</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="D14" s="4">
+        <v>233</v>
+      </c>
+      <c r="E14" s="4">
+        <v>32511</v>
+      </c>
+      <c r="F14" s="4">
+        <v>70476</v>
+      </c>
+      <c r="G14" s="6">
         <v>12</v>
       </c>
-      <c r="E11" s="4">
-        <v>20562</v>
-      </c>
-      <c r="F11" s="4">
-        <v>59286</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5">
-        <v>73</v>
-      </c>
-      <c r="E12" s="5">
-        <v>52958</v>
-      </c>
-      <c r="F12" s="5">
-        <v>131458</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1">
-        <f>SUM(D3:D12)</f>
-        <v>405</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" ref="E13:F13" si="0">SUM(E3:E12)</f>
-        <v>304493</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>797569</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5">
+        <f>SUM(D3:D14)</f>
+        <v>607</v>
+      </c>
+      <c r="E15" s="5">
+        <f>SUM(E3:E14)</f>
+        <v>172912</v>
+      </c>
+      <c r="F15" s="5">
+        <f>SUM(F3:F14)</f>
+        <v>329233</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>